<commit_message>
Add 2023 APWH exam information
</commit_message>
<xml_diff>
--- a/blog/ap-world-history-a-history/ap-world-history-exam-scores.xlsx
+++ b/blog/ap-world-history-a-history/ap-world-history-exam-scores.xlsx
@@ -163,11 +163,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="361323555"/>
-        <c:axId val="938178229"/>
+        <c:axId val="1141306047"/>
+        <c:axId val="1332892949"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="361323555"/>
+        <c:axId val="1141306047"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -219,10 +219,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="938178229"/>
+        <c:crossAx val="1332892949"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="938178229"/>
+        <c:axId val="1332892949"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -297,7 +297,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="361323555"/>
+        <c:crossAx val="1141306047"/>
       </c:valAx>
       <c:lineChart>
         <c:ser>
@@ -455,11 +455,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1408031306"/>
-        <c:axId val="2143564020"/>
+        <c:axId val="2145730656"/>
+        <c:axId val="225185571"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1408031306"/>
+        <c:axId val="2145730656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -483,10 +483,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2143564020"/>
+        <c:crossAx val="225185571"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2143564020"/>
+        <c:axId val="225185571"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -561,7 +561,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1408031306"/>
+        <c:crossAx val="2145730656"/>
         <c:crosses val="max"/>
       </c:valAx>
     </c:plotArea>
@@ -659,11 +659,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="779248093"/>
-        <c:axId val="987851359"/>
+        <c:axId val="1520845574"/>
+        <c:axId val="1185825678"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="779248093"/>
+        <c:axId val="1520845574"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -715,10 +715,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="987851359"/>
+        <c:crossAx val="1185825678"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="987851359"/>
+        <c:axId val="1185825678"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -793,7 +793,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="779248093"/>
+        <c:crossAx val="1520845574"/>
       </c:valAx>
       <c:lineChart>
         <c:varyColors val="0"/>
@@ -828,11 +828,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="2083316371"/>
-        <c:axId val="1508684168"/>
+        <c:axId val="1606059099"/>
+        <c:axId val="2070300465"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2083316371"/>
+        <c:axId val="1606059099"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -856,10 +856,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1508684168"/>
+        <c:crossAx val="2070300465"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1508684168"/>
+        <c:axId val="2070300465"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="3.5"/>
@@ -935,7 +935,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2083316371"/>
+        <c:crossAx val="1606059099"/>
         <c:crosses val="max"/>
       </c:valAx>
     </c:plotArea>
@@ -1821,8 +1821,30 @@
       <c r="I22" s="5"/>
     </row>
     <row r="23">
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
+      <c r="A23" s="3">
+        <v>2023.0</v>
+      </c>
+      <c r="B23" s="3">
+        <v>15.0</v>
+      </c>
+      <c r="C23" s="3">
+        <v>22.0</v>
+      </c>
+      <c r="D23" s="3">
+        <v>28.0</v>
+      </c>
+      <c r="E23" s="3">
+        <v>22.0</v>
+      </c>
+      <c r="F23" s="3">
+        <v>13.0</v>
+      </c>
+      <c r="G23" s="3">
+        <v>3.04</v>
+      </c>
+      <c r="H23" s="3">
+        <v>356000.0</v>
+      </c>
       <c r="I23" s="5"/>
     </row>
   </sheetData>

</xml_diff>